<commit_message>
Alterando pagina da Dashboard
</commit_message>
<xml_diff>
--- a/Tecnologia_da_Informação/documentação/GMUD - VagasIQ.xlsx
+++ b/Tecnologia_da_Informação/documentação/GMUD - VagasIQ.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
   <si>
     <t>REQUISIÇÃO DE MUDANÇA (RFC)</t>
   </si>
@@ -45,7 +45,7 @@
     <t>Data Limite</t>
   </si>
   <si>
-    <t xml:space="preserve">   18/11/2025 ás 02:30</t>
+    <t xml:space="preserve">   18/11/2025 ás 00:30</t>
   </si>
   <si>
     <t>Titulo</t>
@@ -84,7 +84,7 @@
     <t>Tempo Estimado</t>
   </si>
   <si>
-    <t>Tempo previsto de 5 horas de duração.</t>
+    <t>Tempo previsto de 3 horas de duração.</t>
   </si>
   <si>
     <t>Avaliação do Risco</t>
@@ -102,7 +102,7 @@
     <t>Possíveis Impactos</t>
   </si>
   <si>
-    <t>O website pode ficar fora do ar por até 5 horas, tendo um impacto mínimo para os nossos clientes.</t>
+    <t>O website pode ficar fora do ar por até 3 horas, tendo um impacto mínimo para os nossos clientes.</t>
   </si>
   <si>
     <t>Descrição das Tarefas</t>
@@ -120,6 +120,12 @@
     <t>Duração</t>
   </si>
   <si>
+    <t>Início</t>
+  </si>
+  <si>
+    <t>Fim</t>
+  </si>
+  <si>
     <t>Backup da aplicação</t>
   </si>
   <si>
@@ -129,7 +135,7 @@
     <t>Philipi Jordan</t>
   </si>
   <si>
-    <t>01:30 hora</t>
+    <t>30 min</t>
   </si>
   <si>
     <t>Instalar o virtualizador na maquina host da empresa</t>
@@ -141,7 +147,7 @@
     <t>Vitória Lima</t>
   </si>
   <si>
-    <t>30 minutos</t>
+    <t>15 min</t>
   </si>
   <si>
     <t>Fazer configuração para hospedagem da aplicação</t>
@@ -153,13 +159,16 @@
     <t>Heloisy Mota</t>
   </si>
   <si>
-    <t>01:00 hora</t>
-  </si>
-  <si>
     <t>Transferir o website para a máquina virtual</t>
   </si>
   <si>
+    <t>1 hora</t>
+  </si>
+  <si>
     <t>Acessar site via IP, para teste</t>
+  </si>
+  <si>
+    <t>45 min</t>
   </si>
   <si>
     <t>Ferramentas Necessárias</t>
@@ -198,9 +207,6 @@
     <t>Equipe Tecnica</t>
   </si>
   <si>
-    <t>CAB / Comitê de Mudanças</t>
-  </si>
-  <si>
     <t>Responsaveis pelo Teste</t>
   </si>
   <si>
@@ -224,12 +230,27 @@
   <si>
     <t>Vitoria</t>
   </si>
+  <si>
+    <t>Aprovação</t>
+  </si>
+  <si>
+    <t>Comitê de Mudanças</t>
+  </si>
+  <si>
+    <t>Membros</t>
+  </si>
+  <si>
+    <t>Observações Finais</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="13">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="hh:mm"/>
+  </numFmts>
+  <fonts count="12">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -278,17 +299,13 @@
       <name val="Ubuntu"/>
     </font>
     <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
+      <color rgb="FF666666"/>
+      <name val="Ubuntu"/>
     </font>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <color rgb="FF666666"/>
-      <name val="Ubuntu"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -323,7 +340,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="30">
     <border/>
     <border>
       <left style="thin">
@@ -445,17 +462,135 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF1E1E1E"/>
       </left>
       <right style="thin">
         <color rgb="FF1E1E1E"/>
       </right>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="61">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -513,16 +648,23 @@
     <xf borderId="1" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="15" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="17" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="17" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="18" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -535,15 +677,51 @@
     <xf borderId="1" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="19" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="20" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="21" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
+    <xf borderId="22" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="23" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="24" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="25" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="26" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="5" fillId="5" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="27" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="28" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="19" fillId="0" fontId="11" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="9" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="9" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="27" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="29" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="27" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -754,6 +932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1447,11 +1626,15 @@
         <v>28</v>
       </c>
       <c r="I23" s="4"/>
-      <c r="J23" s="26" t="s">
+      <c r="J23" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="K23" s="4"/>
-      <c r="L23" s="27"/>
+      <c r="K23" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="L23" s="27" t="s">
+        <v>31</v>
+      </c>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
@@ -1474,22 +1657,26 @@
         <v>1.0</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="30" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G24" s="8"/>
       <c r="H24" s="30" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I24" s="8"/>
-      <c r="J24" s="30" t="s">
-        <v>33</v>
+      <c r="J24" s="31" t="s">
+        <v>35</v>
       </c>
-      <c r="K24" s="8"/>
-      <c r="L24" s="17"/>
+      <c r="K24" s="32">
+        <v>0.8958333333333334</v>
+      </c>
+      <c r="L24" s="32">
+        <v>0.9166666666666666</v>
+      </c>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
@@ -1515,9 +1702,9 @@
       <c r="G25" s="13"/>
       <c r="H25" s="12"/>
       <c r="I25" s="13"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="17"/>
+      <c r="J25" s="33"/>
+      <c r="K25" s="33"/>
+      <c r="L25" s="33"/>
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
@@ -1540,22 +1727,26 @@
         <v>2.0</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="30" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G26" s="8"/>
       <c r="H26" s="30" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I26" s="8"/>
-      <c r="J26" s="30" t="s">
-        <v>37</v>
+      <c r="J26" s="31" t="s">
+        <v>39</v>
       </c>
-      <c r="K26" s="8"/>
-      <c r="L26" s="17"/>
+      <c r="K26" s="32">
+        <v>0.9166666666666666</v>
+      </c>
+      <c r="L26" s="32">
+        <v>0.9270833333333334</v>
+      </c>
       <c r="M26" s="1"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
@@ -1581,9 +1772,9 @@
       <c r="G27" s="13"/>
       <c r="H27" s="12"/>
       <c r="I27" s="13"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="17"/>
+      <c r="J27" s="33"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="33"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
@@ -1606,22 +1797,26 @@
         <v>3.0</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="30" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G28" s="8"/>
       <c r="H28" s="30" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I28" s="8"/>
-      <c r="J28" s="30" t="s">
-        <v>41</v>
+      <c r="J28" s="31" t="s">
+        <v>35</v>
       </c>
-      <c r="K28" s="8"/>
-      <c r="L28" s="17"/>
+      <c r="K28" s="32">
+        <v>0.9270833333333334</v>
+      </c>
+      <c r="L28" s="32">
+        <v>0.9479166666666666</v>
+      </c>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
@@ -1647,9 +1842,9 @@
       <c r="G29" s="13"/>
       <c r="H29" s="12"/>
       <c r="I29" s="13"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="17"/>
+      <c r="J29" s="33"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="33"/>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
       <c r="O29" s="1"/>
@@ -1672,22 +1867,26 @@
         <v>4.0</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="30" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G30" s="8"/>
       <c r="H30" s="30" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I30" s="8"/>
-      <c r="J30" s="30" t="s">
-        <v>37</v>
+      <c r="J30" s="31" t="s">
+        <v>44</v>
       </c>
-      <c r="K30" s="8"/>
-      <c r="L30" s="17"/>
+      <c r="K30" s="32">
+        <v>0.9479166666666666</v>
+      </c>
+      <c r="L30" s="32">
+        <v>0.9895833333333334</v>
+      </c>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
       <c r="O30" s="1"/>
@@ -1713,9 +1912,9 @@
       <c r="G31" s="13"/>
       <c r="H31" s="12"/>
       <c r="I31" s="13"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="17"/>
+      <c r="J31" s="33"/>
+      <c r="K31" s="33"/>
+      <c r="L31" s="33"/>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
@@ -1738,22 +1937,26 @@
         <v>5.0</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E32" s="8"/>
       <c r="F32" s="30" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G32" s="8"/>
       <c r="H32" s="30" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I32" s="8"/>
-      <c r="J32" s="30" t="s">
-        <v>33</v>
+      <c r="J32" s="31" t="s">
+        <v>46</v>
       </c>
-      <c r="K32" s="8"/>
-      <c r="L32" s="17"/>
+      <c r="K32" s="32">
+        <v>0.9895833333333334</v>
+      </c>
+      <c r="L32" s="32">
+        <v>0.020833333333333332</v>
+      </c>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
       <c r="O32" s="1"/>
@@ -1779,9 +1982,9 @@
       <c r="G33" s="13"/>
       <c r="H33" s="12"/>
       <c r="I33" s="13"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
+      <c r="J33" s="33"/>
+      <c r="K33" s="33"/>
+      <c r="L33" s="33"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
@@ -1800,10 +2003,10 @@
     <row r="34">
       <c r="A34" s="1"/>
       <c r="B34" s="19" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D34" s="10"/>
       <c r="E34" s="10"/>
@@ -1860,28 +2063,28 @@
     <row r="36">
       <c r="A36" s="1"/>
       <c r="B36" s="19" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
-      <c r="C36" s="31" t="s">
-        <v>47</v>
+      <c r="C36" s="34" t="s">
+        <v>50</v>
       </c>
-      <c r="D36" s="32" t="s">
-        <v>48</v>
+      <c r="D36" s="35" t="s">
+        <v>51</v>
       </c>
       <c r="E36" s="4"/>
-      <c r="F36" s="32" t="s">
-        <v>49</v>
+      <c r="F36" s="35" t="s">
+        <v>52</v>
       </c>
       <c r="G36" s="4"/>
-      <c r="H36" s="32" t="s">
-        <v>50</v>
+      <c r="H36" s="35" t="s">
+        <v>53</v>
       </c>
       <c r="I36" s="4"/>
-      <c r="J36" s="32" t="s">
-        <v>51</v>
+      <c r="J36" s="35" t="s">
+        <v>54</v>
       </c>
       <c r="K36" s="4"/>
-      <c r="L36" s="33"/>
+      <c r="L36" s="36"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
@@ -1903,20 +2106,20 @@
       <c r="C37" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="34" t="s">
-        <v>35</v>
+      <c r="D37" s="37" t="s">
+        <v>37</v>
       </c>
       <c r="E37" s="4"/>
-      <c r="F37" s="34" t="s">
-        <v>40</v>
+      <c r="F37" s="37" t="s">
+        <v>42</v>
       </c>
       <c r="G37" s="4"/>
-      <c r="H37" s="34" t="s">
-        <v>31</v>
+      <c r="H37" s="37" t="s">
+        <v>33</v>
       </c>
       <c r="I37" s="4"/>
-      <c r="J37" s="34" t="s">
-        <v>32</v>
+      <c r="J37" s="37" t="s">
+        <v>34</v>
       </c>
       <c r="K37" s="4"/>
       <c r="L37" s="17"/>
@@ -1941,20 +2144,20 @@
       <c r="C38" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D38" s="34" t="s">
-        <v>40</v>
+      <c r="D38" s="37" t="s">
+        <v>42</v>
       </c>
       <c r="E38" s="4"/>
-      <c r="F38" s="34" t="s">
-        <v>39</v>
+      <c r="F38" s="37" t="s">
+        <v>41</v>
       </c>
       <c r="G38" s="4"/>
-      <c r="H38" s="34" t="s">
-        <v>36</v>
+      <c r="H38" s="37" t="s">
+        <v>38</v>
       </c>
       <c r="I38" s="4"/>
-      <c r="J38" s="34" t="s">
-        <v>35</v>
+      <c r="J38" s="37" t="s">
+        <v>37</v>
       </c>
       <c r="K38" s="4"/>
       <c r="L38" s="17"/>
@@ -1976,10 +2179,10 @@
     <row r="39">
       <c r="A39" s="1"/>
       <c r="B39" s="19" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
-      <c r="C39" s="35" t="s">
-        <v>53</v>
+      <c r="C39" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
@@ -2036,28 +2239,26 @@
     <row r="41">
       <c r="A41" s="1"/>
       <c r="B41" s="19" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
-      <c r="C41" s="31" t="s">
-        <v>47</v>
+      <c r="C41" s="34" t="s">
+        <v>50</v>
       </c>
-      <c r="D41" s="32" t="s">
-        <v>55</v>
+      <c r="D41" s="35" t="s">
+        <v>58</v>
       </c>
       <c r="E41" s="4"/>
-      <c r="F41" s="32" t="s">
-        <v>56</v>
+      <c r="F41" s="35" t="s">
+        <v>59</v>
       </c>
       <c r="G41" s="4"/>
-      <c r="H41" s="32" t="s">
-        <v>57</v>
+      <c r="H41" s="35" t="s">
+        <v>60</v>
       </c>
       <c r="I41" s="4"/>
-      <c r="J41" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="K41" s="4"/>
-      <c r="L41" s="36"/>
+      <c r="J41" s="38"/>
+      <c r="K41" s="39"/>
+      <c r="L41" s="40"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
@@ -2075,28 +2276,25 @@
       <c r="A42" s="1"/>
       <c r="B42" s="28"/>
       <c r="C42" s="25" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
-      <c r="D42" s="37" t="b">
+      <c r="D42" s="41" t="b">
         <v>1</v>
       </c>
       <c r="E42" s="4"/>
-      <c r="F42" s="37" t="b">
-        <v>1</v>
+      <c r="F42" s="41" t="b">
+        <v>0</v>
       </c>
       <c r="G42" s="4"/>
-      <c r="H42" s="37" t="b">
+      <c r="H42" s="41" t="b">
         <v>0</v>
       </c>
       <c r="I42" s="4"/>
-      <c r="J42" s="37" t="b">
-        <v>0</v>
-      </c>
-      <c r="K42" s="4"/>
-      <c r="L42" s="17"/>
-      <c r="N42" s="1"/>
-      <c r="O42" s="1"/>
-      <c r="P42" s="1"/>
+      <c r="J42" s="42"/>
+      <c r="L42" s="43"/>
+      <c r="N42" s="15"/>
+      <c r="O42" s="15"/>
+      <c r="P42" s="15"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
       <c r="S42" s="1"/>
@@ -2111,28 +2309,25 @@
       <c r="A43" s="1"/>
       <c r="B43" s="28"/>
       <c r="C43" s="25" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
-      <c r="D43" s="37" t="b">
+      <c r="D43" s="41" t="b">
         <v>1</v>
       </c>
       <c r="E43" s="4"/>
-      <c r="F43" s="37" t="b">
-        <v>1</v>
+      <c r="F43" s="41" t="b">
+        <v>0</v>
       </c>
       <c r="G43" s="4"/>
-      <c r="H43" s="37" t="b">
+      <c r="H43" s="41" t="b">
         <v>0</v>
       </c>
       <c r="I43" s="4"/>
-      <c r="J43" s="37" t="b">
-        <v>0</v>
-      </c>
-      <c r="K43" s="4"/>
-      <c r="L43" s="17"/>
-      <c r="N43" s="1"/>
-      <c r="O43" s="1"/>
-      <c r="P43" s="1"/>
+      <c r="J43" s="42"/>
+      <c r="L43" s="43"/>
+      <c r="N43" s="15"/>
+      <c r="O43" s="15"/>
+      <c r="P43" s="15"/>
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
@@ -2147,28 +2342,24 @@
       <c r="A44" s="1"/>
       <c r="B44" s="28"/>
       <c r="C44" s="25" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
-      <c r="D44" s="37" t="b">
+      <c r="D44" s="41" t="b">
         <v>1</v>
       </c>
       <c r="E44" s="4"/>
-      <c r="F44" s="37" t="b">
+      <c r="F44" s="41" t="b">
         <v>1</v>
       </c>
       <c r="G44" s="4"/>
-      <c r="H44" s="37" t="b">
-        <v>1</v>
+      <c r="H44" s="41" t="b">
+        <v>0</v>
       </c>
       <c r="I44" s="4"/>
-      <c r="J44" s="37" t="b">
-        <v>0</v>
-      </c>
-      <c r="K44" s="4"/>
-      <c r="L44" s="17"/>
-      <c r="N44" s="1"/>
-      <c r="O44" s="1"/>
-      <c r="P44" s="1"/>
+      <c r="J44" s="42"/>
+      <c r="L44" s="43"/>
+      <c r="N44" s="15"/>
+      <c r="O44" s="44"/>
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
@@ -2183,28 +2374,24 @@
       <c r="A45" s="1"/>
       <c r="B45" s="28"/>
       <c r="C45" s="25" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
-      <c r="D45" s="37" t="b">
+      <c r="D45" s="41" t="b">
         <v>1</v>
       </c>
       <c r="E45" s="4"/>
-      <c r="F45" s="37" t="b">
-        <v>1</v>
+      <c r="F45" s="41" t="b">
+        <v>0</v>
       </c>
       <c r="G45" s="4"/>
-      <c r="H45" s="37" t="b">
+      <c r="H45" s="41" t="b">
         <v>0</v>
       </c>
       <c r="I45" s="4"/>
-      <c r="J45" s="37" t="b">
-        <v>0</v>
-      </c>
-      <c r="K45" s="4"/>
-      <c r="L45" s="17"/>
-      <c r="N45" s="1"/>
-      <c r="O45" s="1"/>
-      <c r="P45" s="1"/>
+      <c r="J45" s="42"/>
+      <c r="L45" s="43"/>
+      <c r="N45" s="15"/>
+      <c r="O45" s="45"/>
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
@@ -2219,28 +2406,24 @@
       <c r="A46" s="1"/>
       <c r="B46" s="28"/>
       <c r="C46" s="25" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
-      <c r="D46" s="37" t="b">
+      <c r="D46" s="41" t="b">
         <v>1</v>
       </c>
       <c r="E46" s="4"/>
-      <c r="F46" s="37" t="b">
+      <c r="F46" s="41" t="b">
         <v>1</v>
       </c>
       <c r="G46" s="4"/>
-      <c r="H46" s="37" t="b">
-        <v>1</v>
+      <c r="H46" s="41" t="b">
+        <v>0</v>
       </c>
       <c r="I46" s="4"/>
-      <c r="J46" s="37" t="b">
-        <v>0</v>
-      </c>
-      <c r="K46" s="4"/>
-      <c r="L46" s="17"/>
-      <c r="N46" s="1"/>
-      <c r="O46" s="1"/>
-      <c r="P46" s="1"/>
+      <c r="J46" s="42"/>
+      <c r="L46" s="43"/>
+      <c r="N46" s="15"/>
+      <c r="O46" s="45"/>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>
@@ -2255,28 +2438,25 @@
       <c r="A47" s="1"/>
       <c r="B47" s="11"/>
       <c r="C47" s="25" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
-      <c r="D47" s="37" t="b">
+      <c r="D47" s="41" t="b">
         <v>1</v>
       </c>
       <c r="E47" s="4"/>
-      <c r="F47" s="37" t="b">
+      <c r="F47" s="41" t="b">
+        <v>0</v>
+      </c>
+      <c r="G47" s="4"/>
+      <c r="H47" s="41" t="b">
         <v>1</v>
       </c>
-      <c r="G47" s="4"/>
-      <c r="H47" s="37" t="b">
-        <v>0</v>
-      </c>
       <c r="I47" s="4"/>
-      <c r="J47" s="37" t="b">
-        <v>1</v>
-      </c>
-      <c r="K47" s="4"/>
-      <c r="L47" s="17"/>
-      <c r="N47" s="1"/>
-      <c r="O47" s="1"/>
-      <c r="P47" s="1"/>
+      <c r="J47" s="46"/>
+      <c r="K47" s="47"/>
+      <c r="L47" s="48"/>
+      <c r="N47" s="15"/>
+      <c r="O47" s="45"/>
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
       <c r="S47" s="1"/>
@@ -2289,12 +2469,12 @@
     </row>
     <row r="48">
       <c r="A48" s="1"/>
-      <c r="K48" s="1"/>
-      <c r="L48" s="1"/>
+      <c r="B48" s="49" t="s">
+        <v>67</v>
+      </c>
       <c r="M48" s="1"/>
-      <c r="N48" s="1"/>
-      <c r="O48" s="1"/>
-      <c r="P48" s="1"/>
+      <c r="N48" s="15"/>
+      <c r="O48" s="45"/>
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
       <c r="S48" s="1"/>
@@ -2308,12 +2488,26 @@
     </row>
     <row r="49">
       <c r="A49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="L49" s="1"/>
+      <c r="B49" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="C49" s="51" t="s">
+        <v>69</v>
+      </c>
+      <c r="D49" s="52"/>
+      <c r="E49" s="51" t="s">
+        <v>67</v>
+      </c>
+      <c r="F49" s="52"/>
+      <c r="G49" s="53"/>
+      <c r="H49" s="39"/>
+      <c r="I49" s="39"/>
+      <c r="J49" s="39"/>
+      <c r="K49" s="39"/>
+      <c r="L49" s="40"/>
       <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
-      <c r="O49" s="1"/>
-      <c r="P49" s="1"/>
+      <c r="N49" s="15"/>
+      <c r="O49" s="45"/>
       <c r="Q49" s="1"/>
       <c r="R49" s="1"/>
       <c r="S49" s="1"/>
@@ -2327,12 +2521,20 @@
     </row>
     <row r="50">
       <c r="A50" s="1"/>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="D50" s="13"/>
+      <c r="E50" s="55" t="b">
+        <v>1</v>
+      </c>
+      <c r="F50" s="13"/>
+      <c r="G50" s="42"/>
+      <c r="L50" s="43"/>
       <c r="M50" s="1"/>
-      <c r="N50" s="1"/>
-      <c r="O50" s="1"/>
-      <c r="P50" s="1"/>
+      <c r="N50" s="15"/>
+      <c r="O50" s="45"/>
       <c r="Q50" s="1"/>
       <c r="R50" s="1"/>
       <c r="S50" s="1"/>
@@ -2346,12 +2548,21 @@
     </row>
     <row r="51">
       <c r="A51" s="1"/>
-      <c r="K51" s="1"/>
-      <c r="L51" s="1"/>
+      <c r="B51" s="16"/>
+      <c r="C51" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="D51" s="4"/>
+      <c r="E51" s="41" t="b">
+        <v>1</v>
+      </c>
+      <c r="F51" s="4"/>
+      <c r="G51" s="42"/>
+      <c r="L51" s="43"/>
       <c r="M51" s="1"/>
-      <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
-      <c r="P51" s="1"/>
+      <c r="N51" s="15"/>
+      <c r="O51" s="15"/>
+      <c r="P51" s="15"/>
       <c r="Q51" s="1"/>
       <c r="R51" s="1"/>
       <c r="S51" s="1"/>
@@ -2365,8 +2576,17 @@
     </row>
     <row r="52">
       <c r="A52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="37" t="s">
+        <v>63</v>
+      </c>
+      <c r="D52" s="4"/>
+      <c r="E52" s="41" t="b">
+        <v>1</v>
+      </c>
+      <c r="F52" s="4"/>
+      <c r="G52" s="42"/>
+      <c r="L52" s="43"/>
       <c r="M52" s="1"/>
       <c r="N52" s="1"/>
       <c r="O52" s="1"/>
@@ -2384,8 +2604,17 @@
     </row>
     <row r="53">
       <c r="A53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
+      <c r="B53" s="16"/>
+      <c r="C53" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="D53" s="4"/>
+      <c r="E53" s="41" t="b">
+        <v>1</v>
+      </c>
+      <c r="F53" s="4"/>
+      <c r="G53" s="42"/>
+      <c r="L53" s="43"/>
       <c r="M53" s="1"/>
       <c r="N53" s="1"/>
       <c r="O53" s="1"/>
@@ -2403,8 +2632,17 @@
     </row>
     <row r="54">
       <c r="A54" s="1"/>
-      <c r="K54" s="1"/>
-      <c r="L54" s="1"/>
+      <c r="B54" s="16"/>
+      <c r="C54" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="D54" s="4"/>
+      <c r="E54" s="41" t="b">
+        <v>1</v>
+      </c>
+      <c r="F54" s="4"/>
+      <c r="G54" s="42"/>
+      <c r="L54" s="43"/>
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
       <c r="O54" s="1"/>
@@ -2422,8 +2660,21 @@
     </row>
     <row r="55">
       <c r="A55" s="1"/>
-      <c r="K55" s="1"/>
-      <c r="L55" s="1"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="56" t="s">
+        <v>66</v>
+      </c>
+      <c r="D55" s="8"/>
+      <c r="E55" s="57" t="b">
+        <v>1</v>
+      </c>
+      <c r="F55" s="8"/>
+      <c r="G55" s="46"/>
+      <c r="H55" s="47"/>
+      <c r="I55" s="47"/>
+      <c r="J55" s="47"/>
+      <c r="K55" s="47"/>
+      <c r="L55" s="48"/>
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
       <c r="O55" s="1"/>
@@ -2441,8 +2692,19 @@
     </row>
     <row r="56">
       <c r="A56" s="1"/>
-      <c r="K56" s="1"/>
-      <c r="L56" s="1"/>
+      <c r="B56" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" s="59"/>
+      <c r="D56" s="59"/>
+      <c r="E56" s="59"/>
+      <c r="F56" s="59"/>
+      <c r="G56" s="59"/>
+      <c r="H56" s="59"/>
+      <c r="I56" s="59"/>
+      <c r="J56" s="59"/>
+      <c r="K56" s="59"/>
+      <c r="L56" s="52"/>
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
       <c r="O56" s="1"/>
@@ -2460,17 +2722,17 @@
     </row>
     <row r="57">
       <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="1"/>
-      <c r="J57" s="1"/>
-      <c r="K57" s="1"/>
-      <c r="L57" s="1"/>
+      <c r="B57" s="60"/>
+      <c r="C57" s="59"/>
+      <c r="D57" s="59"/>
+      <c r="E57" s="59"/>
+      <c r="F57" s="59"/>
+      <c r="G57" s="59"/>
+      <c r="H57" s="59"/>
+      <c r="I57" s="59"/>
+      <c r="J57" s="59"/>
+      <c r="K57" s="59"/>
+      <c r="L57" s="52"/>
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
       <c r="O57" s="1"/>
@@ -28527,117 +28789,147 @@
       <c r="Z987" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="109">
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="D30:E31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D28:E29"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="B23:B33"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="D32:E33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="D44:E44"/>
+  <mergeCells count="136">
     <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="F24:G25"/>
-    <mergeCell ref="F28:G29"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F30:G31"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="D13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="B41:B47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="F32:G33"/>
     <mergeCell ref="D26:E27"/>
-    <mergeCell ref="D24:E25"/>
-    <mergeCell ref="J32:K33"/>
-    <mergeCell ref="H32:I33"/>
-    <mergeCell ref="H24:I25"/>
-    <mergeCell ref="H23:I23"/>
     <mergeCell ref="F26:G27"/>
     <mergeCell ref="H26:I27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:E29"/>
+    <mergeCell ref="F28:G29"/>
+    <mergeCell ref="H28:I29"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="L28:L29"/>
+    <mergeCell ref="D32:E33"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="F32:G33"/>
+    <mergeCell ref="H32:I33"/>
+    <mergeCell ref="J32:J33"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="L32:L33"/>
+    <mergeCell ref="C34:L35"/>
+    <mergeCell ref="D30:E31"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="F30:G31"/>
     <mergeCell ref="H30:I31"/>
-    <mergeCell ref="H28:I29"/>
-    <mergeCell ref="J30:K31"/>
-    <mergeCell ref="L23:L33"/>
-    <mergeCell ref="J28:K29"/>
-    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="L30:L31"/>
+    <mergeCell ref="L36:L38"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="O44:P44"/>
+    <mergeCell ref="O45:P45"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="O46:P46"/>
+    <mergeCell ref="O47:P47"/>
+    <mergeCell ref="O48:P48"/>
+    <mergeCell ref="O49:P49"/>
+    <mergeCell ref="O50:P50"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="C39:L40"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:L47"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B41:B47"/>
+    <mergeCell ref="B48:L48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="G49:L55"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="B3:L3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:D5"/>
+    <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:G5"/>
-    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="H4:L5"/>
+    <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:L7"/>
-    <mergeCell ref="H4:L5"/>
+    <mergeCell ref="B8:B9"/>
     <mergeCell ref="C8:L9"/>
     <mergeCell ref="B10:L10"/>
-    <mergeCell ref="G13:H14"/>
+    <mergeCell ref="B11:B12"/>
     <mergeCell ref="C11:L12"/>
     <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:H14"/>
+    <mergeCell ref="I13:I14"/>
     <mergeCell ref="J13:K14"/>
     <mergeCell ref="L13:L14"/>
     <mergeCell ref="C15:L16"/>
-    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="C17:L18"/>
     <mergeCell ref="C19:L20"/>
     <mergeCell ref="C21:L22"/>
-    <mergeCell ref="C17:L18"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="L41:L47"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="J26:K27"/>
-    <mergeCell ref="J24:K25"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="C34:L35"/>
-    <mergeCell ref="C39:L40"/>
-    <mergeCell ref="L36:L38"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:E25"/>
+    <mergeCell ref="F24:G25"/>
+    <mergeCell ref="H24:I25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B49:B55"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="B56:L56"/>
+    <mergeCell ref="B57:L57"/>
   </mergeCells>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>